<commit_message>
trying to prepare the data: reading parameters from excel to transform then into AMPL impunt
</commit_message>
<xml_diff>
--- a/notebooks/model_data.xlsx
+++ b/notebooks/model_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\storreglosa\Projects\05_Multimodal_Logistics_Network\multimodal_logistics_network_colombia\multimodal_logistics_network_colombia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\storreglosa\Projects\05_Multimodal_Logistics_Network\multimodal_logistics_network_colombia\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6293DCC6-A68C-453A-9FEB-F99B94890CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9BF358-8E91-4498-AE1D-D31A6B515705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fk" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="56">
   <si>
     <t>ctl_bogota</t>
   </si>
@@ -185,6 +185,30 @@
   </si>
   <si>
     <t>CAPm</t>
+  </si>
+  <si>
+    <t>code_inicio_type</t>
+  </si>
+  <si>
+    <t>code_fin_type</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>PCTL</t>
   </si>
 </sst>
 </file>
@@ -554,9 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4043D3F5-E123-4311-B3BA-8D9F206DCE89}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -653,9 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254CA286-5D4A-4576-99A9-A6F35DAB07FE}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -665,7 +685,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
@@ -816,7 +836,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +847,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>47</v>
@@ -869,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{830C797F-F77F-42C5-B05F-4D395FB93FC6}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +919,7 @@
       </c>
       <c r="C2" s="6">
         <f ca="1">INT(RAND()*500)</f>
-        <v>472</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,7 +932,7 @@
       </c>
       <c r="C3" s="6">
         <f t="shared" ref="C3:C49" ca="1" si="1">INT(RAND()*500)</f>
-        <v>302</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -925,7 +945,7 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>208</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -938,7 +958,7 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>388</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -951,7 +971,7 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>397</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -964,7 +984,7 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>487</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -977,7 +997,7 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>448</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -990,7 +1010,7 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>471</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,7 +1022,7 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>434</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,7 +1035,7 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>393</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1028,7 +1048,7 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>124</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1041,7 +1061,7 @@
       </c>
       <c r="C13" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>461</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1054,7 +1074,7 @@
       </c>
       <c r="C14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>193</v>
+        <v>443</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,7 +1087,7 @@
       </c>
       <c r="C15" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>151</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1080,7 +1100,7 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,7 +1113,7 @@
       </c>
       <c r="C17" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>141</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1105,7 +1125,7 @@
       </c>
       <c r="C18" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>482</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1118,7 +1138,7 @@
       </c>
       <c r="C19" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>269</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1131,7 +1151,7 @@
       </c>
       <c r="C20" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>62</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,7 +1164,7 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>313</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,7 +1177,7 @@
       </c>
       <c r="C22" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>365</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,7 +1190,7 @@
       </c>
       <c r="C23" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>134</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1183,7 +1203,7 @@
       </c>
       <c r="C24" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>454</v>
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,7 +1216,7 @@
       </c>
       <c r="C25" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>130</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,7 +1228,7 @@
       </c>
       <c r="C26" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>424</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1221,7 +1241,7 @@
       </c>
       <c r="C27" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1234,7 +1254,7 @@
       </c>
       <c r="C28" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,7 +1267,7 @@
       </c>
       <c r="C29" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>348</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1260,7 +1280,7 @@
       </c>
       <c r="C30" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>122</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1273,7 +1293,7 @@
       </c>
       <c r="C31" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>208</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1286,7 +1306,7 @@
       </c>
       <c r="C32" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>411</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1299,7 +1319,7 @@
       </c>
       <c r="C33" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1311,7 +1331,7 @@
       </c>
       <c r="C34" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>388</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1324,7 +1344,7 @@
       </c>
       <c r="C35" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>117</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1337,7 +1357,7 @@
       </c>
       <c r="C36" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>485</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,7 +1370,7 @@
       </c>
       <c r="C37" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>225</v>
+        <v>487</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1363,7 +1383,7 @@
       </c>
       <c r="C38" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>170</v>
+        <v>452</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1376,7 +1396,7 @@
       </c>
       <c r="C39" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>53</v>
+        <v>463</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1389,7 +1409,7 @@
       </c>
       <c r="C40" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1402,7 +1422,7 @@
       </c>
       <c r="C41" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>431</v>
+        <v>455</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1414,7 +1434,7 @@
       </c>
       <c r="C42" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>240</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1427,7 +1447,7 @@
       </c>
       <c r="C43" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>459</v>
+        <v>396</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1440,7 +1460,7 @@
       </c>
       <c r="C44" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>498</v>
+        <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,7 +1473,7 @@
       </c>
       <c r="C45" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>444</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1466,7 +1486,7 @@
       </c>
       <c r="C46" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>328</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1479,7 +1499,7 @@
       </c>
       <c r="C47" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1492,7 +1512,7 @@
       </c>
       <c r="C48" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>359</v>
+        <v>322</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1505,7 +1525,7 @@
       </c>
       <c r="C49" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -1515,19 +1535,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E1AA60-99B0-440F-963B-1E73FB5FCB8F}">
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:F124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.85546875" customWidth="1"/>
+    <col min="1" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1535,1731 +1555,2475 @@
         <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7">
         <v>5641.6</v>
       </c>
-      <c r="D2" s="7">
+      <c r="F2" s="7">
         <v>2840.1634800000002</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="7">
         <v>27714.933333333334</v>
       </c>
-      <c r="D3" s="7">
+      <c r="F3" s="7">
         <v>13952.59173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="7">
         <v>20353.333333333332</v>
       </c>
-      <c r="D4" s="7">
+      <c r="F4" s="7">
         <v>10246.52475</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="7">
         <v>86435.733333333337</v>
       </c>
-      <c r="D5" s="7">
+      <c r="F5" s="7">
         <v>43514.537219999998</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="7">
         <v>100654.39999999999</v>
       </c>
-      <c r="D6" s="7">
+      <c r="F6" s="7">
         <v>50672.67282</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="7">
         <v>18289.333333333332</v>
       </c>
-      <c r="D7" s="7">
+      <c r="F7" s="7">
         <v>9207.4405500000012</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="7">
         <v>28345.599999999999</v>
       </c>
-      <c r="D8" s="7">
+      <c r="F8" s="7">
         <v>14270.089680000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="7">
         <v>19963.466666666667</v>
       </c>
-      <c r="D9" s="7">
+      <c r="F9" s="7">
         <v>10050.253289999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="7">
         <v>99507.733333333337</v>
       </c>
-      <c r="D10" s="7">
+      <c r="F10" s="7">
         <v>50095.40382</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="7">
         <v>85243.199999999997</v>
       </c>
-      <c r="D11" s="7">
+      <c r="F11" s="7">
         <v>42914.177459999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="7">
         <v>18874.133333333335</v>
       </c>
-      <c r="D12" s="7">
+      <c r="F12" s="7">
         <v>9501.8477399999992</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="7">
         <v>28746.933333333334</v>
       </c>
-      <c r="D13" s="7">
+      <c r="F13" s="7">
         <v>14472.133830000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="7">
         <v>19837.333333333332</v>
       </c>
-      <c r="D14" s="7">
+      <c r="F14" s="7">
         <v>9986.7537000000011</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="7">
         <v>98808.266666666663</v>
       </c>
-      <c r="D15" s="7">
+      <c r="F15" s="7">
         <v>49743.26973</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="7">
         <v>19493.333333333332</v>
       </c>
-      <c r="D16" s="7">
+      <c r="F16" s="7">
         <v>9813.5730000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="7">
         <v>84474.933333333334</v>
       </c>
-      <c r="D17" s="7">
+      <c r="F17" s="7">
         <v>42527.407229999997</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="7">
         <v>6742.4</v>
       </c>
-      <c r="D18" s="7">
+      <c r="F18" s="7">
         <v>3394.3417199999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="7">
         <v>7499.2</v>
       </c>
-      <c r="D19" s="7">
+      <c r="F19" s="7">
         <v>3775.3392600000006</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="7">
         <v>45.333333333333336</v>
       </c>
-      <c r="D20" s="7">
+      <c r="F20" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="7">
         <v>45.333333333333336</v>
       </c>
-      <c r="D21" s="7">
+      <c r="F21" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="7">
         <v>45.333333333333336</v>
       </c>
-      <c r="D22" s="7">
+      <c r="F22" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="7">
         <v>119.29719777777778</v>
       </c>
-      <c r="D23" s="7">
+      <c r="F23" s="7">
         <v>41.274999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7">
         <v>132.22337933333336</v>
       </c>
-      <c r="D24" s="7">
+      <c r="F24" s="7">
         <v>59.994999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="7">
         <v>479.32466666666664</v>
       </c>
-      <c r="D25" s="7">
+      <c r="F25" s="7">
         <v>258.04999999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="7">
         <v>306.70448222222223</v>
       </c>
-      <c r="D26" s="7">
+      <c r="F26" s="7">
         <v>125.44999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="7">
         <v>343.04289777777774</v>
       </c>
-      <c r="D27" s="7">
+      <c r="F27" s="7">
         <v>140.39999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="7">
         <v>254.21130444444441</v>
       </c>
-      <c r="D28" s="7">
+      <c r="F28" s="7">
         <v>112.45</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="7">
         <v>324.62826666666666</v>
       </c>
-      <c r="D29" s="7">
+      <c r="F29" s="7">
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="7">
         <v>265.68207777777781</v>
       </c>
-      <c r="D30" s="7">
+      <c r="F30" s="7">
         <v>111.14999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="7">
         <v>214.78685999999999</v>
       </c>
-      <c r="D31" s="7">
+      <c r="F31" s="7">
         <v>104.65</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="7">
         <v>46.222222222222221</v>
       </c>
-      <c r="D32" s="7">
+      <c r="F32" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="7">
         <v>334.8029377777778</v>
       </c>
-      <c r="D33" s="7">
+      <c r="F33" s="7">
         <v>222.29999999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="7">
         <v>333.82918000000001</v>
       </c>
-      <c r="D34" s="7">
+      <c r="F34" s="7">
         <v>221.64999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="7">
         <v>533.38610000000006</v>
       </c>
-      <c r="D35" s="7">
+      <c r="F35" s="7">
         <v>342.55</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="7">
         <v>359.36931111111113</v>
       </c>
-      <c r="D36" s="7">
+      <c r="F36" s="7">
         <v>217.1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="7">
         <v>428.85418222222222</v>
       </c>
-      <c r="D37" s="7">
+      <c r="F37" s="7">
         <v>250.89999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="7">
         <v>370.63932444444441</v>
       </c>
-      <c r="D38" s="7">
+      <c r="F38" s="7">
         <v>218.39999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="7">
         <v>187.84571111111111</v>
       </c>
-      <c r="D39" s="7">
+      <c r="F39" s="7">
         <v>107.25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="7">
         <v>7.2349311111111119</v>
       </c>
-      <c r="D40" s="7">
+      <c r="F40" s="7">
         <v>2.2749999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E41" s="7">
         <v>362.22425111111113</v>
       </c>
-      <c r="D41" s="7">
+      <c r="F41" s="7">
         <v>187.85</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E42" s="7">
         <v>403.58549777777779</v>
       </c>
-      <c r="D42" s="7">
+      <c r="F42" s="7">
         <v>209.3</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="7">
         <v>455.9546866666667</v>
       </c>
-      <c r="D43" s="7">
+      <c r="F43" s="7">
         <v>246.34999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E44" s="7">
         <v>401.81758666666667</v>
       </c>
-      <c r="D44" s="7">
+      <c r="F44" s="7">
         <v>217.1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="7">
         <v>44.444444444444443</v>
       </c>
-      <c r="D45" s="7">
+      <c r="F45" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="7">
         <v>253.41247333333331</v>
       </c>
-      <c r="D46" s="7">
+      <c r="F46" s="7">
         <v>115.04999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="7">
         <v>220.28799999999998</v>
       </c>
-      <c r="D47" s="7">
+      <c r="F47" s="7">
         <v>77.999999999999986</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E48" s="7">
         <v>289.06031777777775</v>
       </c>
-      <c r="D48" s="7">
+      <c r="F48" s="7">
         <v>112.45</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="7">
         <v>287.77348666666666</v>
       </c>
-      <c r="D49" s="7">
+      <c r="F49" s="7">
         <v>130.65</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E50" s="7">
         <v>252.43352666666664</v>
       </c>
-      <c r="D50" s="7">
+      <c r="F50" s="7">
         <v>112.45</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="7">
         <v>358.66216666666674</v>
       </c>
-      <c r="D51" s="7">
+      <c r="F51" s="7">
         <v>217.74999999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E52" s="7">
         <v>44.444444444444443</v>
       </c>
-      <c r="D52" s="7">
+      <c r="F52" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E53" s="7">
         <v>145.78983199999999</v>
       </c>
-      <c r="D53" s="7">
+      <c r="F53" s="7">
         <v>34.709999999999994</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="7">
         <v>207.43786666666665</v>
       </c>
-      <c r="D54" s="7">
+      <c r="F54" s="7">
         <v>73.449999999999989</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" s="7">
         <v>322.85048888888889</v>
       </c>
-      <c r="D55" s="7">
+      <c r="F55" s="7">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" s="7">
         <v>422.65074222222216</v>
       </c>
-      <c r="D56" s="7">
+      <c r="F56" s="7">
         <v>248.3</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="7">
         <v>388.42453333333333</v>
       </c>
-      <c r="D57" s="7">
+      <c r="F57" s="7">
         <v>191.75</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" s="7">
         <v>417.39178666666669</v>
       </c>
-      <c r="D58" s="7">
+      <c r="F58" s="7">
         <v>206.04999999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" s="7">
         <v>44.444444444444443</v>
       </c>
-      <c r="D59" s="7">
+      <c r="F59" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="7">
         <v>145.51681733333334</v>
       </c>
-      <c r="D60" s="7">
+      <c r="F60" s="7">
         <v>34.644999999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="7">
         <v>274.0224977777778</v>
       </c>
-      <c r="D61" s="7">
+      <c r="F61" s="7">
         <v>106.60000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E62" s="7">
         <v>421.56644444444447</v>
       </c>
-      <c r="D62" s="7">
+      <c r="F62" s="7">
         <v>200.2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" s="7">
         <v>401.03561111111111</v>
       </c>
-      <c r="D63" s="7">
+      <c r="F63" s="7">
         <v>190.45</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="7">
         <v>263.90430000000003</v>
       </c>
-      <c r="D64" s="7">
+      <c r="F64" s="7">
         <v>111.14999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="7">
         <v>365.56813999999997</v>
       </c>
-      <c r="D65" s="7">
+      <c r="F65" s="7">
         <v>216.45</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66" s="7">
         <v>44.444444444444443</v>
       </c>
-      <c r="D66" s="7">
+      <c r="F66" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" s="7">
         <v>119.98662533333334</v>
       </c>
-      <c r="D67" s="7">
+      <c r="F67" s="7">
         <v>18.265000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="7">
         <v>292.06861333333336</v>
       </c>
-      <c r="D68" s="7">
+      <c r="F68" s="7">
         <v>132.6</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E69" s="7">
         <v>420.02517333333333</v>
       </c>
-      <c r="D69" s="7">
+      <c r="F69" s="7">
         <v>207.35000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" s="7">
         <v>409.39238666666665</v>
       </c>
-      <c r="D70" s="7">
+      <c r="F70" s="7">
         <v>191.1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E71" s="7">
         <v>304.92670444444445</v>
       </c>
-      <c r="D71" s="7">
+      <c r="F71" s="7">
         <v>125.44999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E72" s="7">
         <v>401.32617777777779</v>
       </c>
-      <c r="D72" s="7">
+      <c r="F72" s="7">
         <v>219.70000000000002</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" s="7">
         <v>262.61381999999998</v>
       </c>
-      <c r="D73" s="7">
+      <c r="F73" s="7">
         <v>111.14999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E74" s="7">
         <v>349.20846444444442</v>
       </c>
-      <c r="D74" s="7">
+      <c r="F74" s="7">
         <v>156.65</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="7">
         <v>518.84159333333332</v>
       </c>
-      <c r="D75" s="7">
+      <c r="F75" s="7">
         <v>271.04999999999995</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E76" s="7">
         <v>539.99340888888901</v>
       </c>
-      <c r="D76" s="7">
+      <c r="F76" s="7">
         <v>282.09999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E77" s="7">
         <v>440.4291622222222</v>
       </c>
-      <c r="D77" s="7">
+      <c r="F77" s="7">
         <v>209.95</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E78" s="7">
         <v>296.62204444444444</v>
       </c>
-      <c r="D78" s="7">
+      <c r="F78" s="7">
         <v>127.4</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E79" s="7">
         <v>324.31807111111107</v>
       </c>
-      <c r="D79" s="7">
+      <c r="F79" s="7">
         <v>137.79999999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="7">
         <v>256.36426666666671</v>
       </c>
-      <c r="D80" s="7">
+      <c r="F80" s="7">
         <v>136.5</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="7">
         <v>716.99768888888889</v>
       </c>
-      <c r="D81" s="7">
+      <c r="F81" s="7">
         <v>416</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="7">
         <v>767.45445333333339</v>
       </c>
-      <c r="D82" s="7">
+      <c r="F82" s="7">
         <v>452.4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="7">
         <v>848.12970666666661</v>
       </c>
-      <c r="D83" s="7">
+      <c r="F83" s="7">
         <v>540.79999999999995</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E84" s="7">
         <v>615.37309555555544</v>
       </c>
-      <c r="D84" s="7">
+      <c r="F84" s="7">
         <v>404.95</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="7">
         <v>623.10424444444448</v>
       </c>
-      <c r="D85" s="7">
+      <c r="F85" s="7">
         <v>383.5</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="7">
         <v>554.98594666666668</v>
       </c>
-      <c r="D86" s="7">
+      <c r="F86" s="7">
         <v>354.9</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="7">
         <v>615.37309555555544</v>
       </c>
-      <c r="D87" s="7">
+      <c r="F87" s="7">
         <v>404.95</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C88" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="7">
         <v>967.11027555555563</v>
       </c>
-      <c r="D88" s="7">
+      <c r="F88" s="7">
         <v>653.9</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C89" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89" s="7">
         <v>895.98320000000001</v>
       </c>
-      <c r="D89" s="7">
+      <c r="F89" s="7">
         <v>627.25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" s="7">
         <v>103.36819844444446</v>
       </c>
-      <c r="D90" s="7">
+      <c r="F90" s="7">
         <v>16.704999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" s="7">
         <v>44.444444444444443</v>
       </c>
-      <c r="D91" s="7">
+      <c r="F91" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C92" s="7">
+      <c r="C92" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="7">
         <v>349.16477555555554</v>
       </c>
-      <c r="D92" s="7">
+      <c r="F92" s="7">
         <v>143.64999999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C93" s="7">
+      <c r="C93" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E93" s="7">
         <v>450.0077555555556</v>
       </c>
-      <c r="D93" s="7">
+      <c r="F93" s="7">
         <v>246.34999999999997</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="7">
+      <c r="C94" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="7">
         <v>1054.9253066666665</v>
       </c>
-      <c r="D94" s="7">
+      <c r="F94" s="7">
         <v>694.19999999999993</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="7">
+      <c r="C95" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E95" s="7">
         <v>1014.2160444444445</v>
       </c>
-      <c r="D95" s="7">
+      <c r="F95" s="7">
         <v>685.75</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C96" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="7">
         <v>940.55024000000003</v>
       </c>
-      <c r="D96" s="7">
+      <c r="F96" s="7">
         <v>658.44999999999993</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C97" s="7">
+      <c r="C97" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E97" s="7">
         <v>904.40876000000003</v>
       </c>
-      <c r="D97" s="7">
+      <c r="F97" s="7">
         <v>553.15</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="7">
+      <c r="C98" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E98" s="7">
         <v>957.57028888888885</v>
       </c>
-      <c r="D98" s="7">
+      <c r="F98" s="7">
         <v>589.54999999999995</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C99" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E99" s="7">
         <v>967.43816888888909</v>
       </c>
-      <c r="D99" s="7">
+      <c r="F99" s="7">
         <v>655.84999999999991</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C100" s="7">
+      <c r="C100" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100" s="7">
         <v>980.82771111111117</v>
       </c>
-      <c r="D100" s="7">
+      <c r="F100" s="7">
         <v>679.25</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C101" s="7">
+      <c r="C101" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" s="7">
         <v>936.56776888888885</v>
       </c>
-      <c r="D101" s="7">
+      <c r="F101" s="7">
         <v>657.8</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C102" s="7">
+      <c r="C102" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E102" s="7">
         <v>911.70731111111104</v>
       </c>
-      <c r="D102" s="7">
+      <c r="F102" s="7">
         <v>630.5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="7">
+      <c r="C103" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E103" s="7">
         <v>1110.8720000000003</v>
       </c>
-      <c r="D103" s="7">
+      <c r="F103" s="7">
         <v>780</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C104" s="7">
+      <c r="C104" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E104" s="7">
         <v>1089.7912799999999</v>
       </c>
-      <c r="D104" s="7">
+      <c r="F104" s="7">
         <v>758.55</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C105" s="7">
+      <c r="C105" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E105" s="7">
         <v>1046.0445533333334</v>
       </c>
-      <c r="D105" s="7">
+      <c r="F105" s="7">
         <v>729.95</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C106" s="7">
+      <c r="C106" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E106" s="7">
         <v>871.86915999999997</v>
       </c>
-      <c r="D106" s="7">
+      <c r="F106" s="7">
         <v>542.09999999999991</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="7">
+      <c r="C107" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E107" s="7">
         <v>923.38291111111118</v>
       </c>
-      <c r="D107" s="7">
+      <c r="F107" s="7">
         <v>578.5</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C108" s="7">
+      <c r="C108" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108" s="7">
         <v>906.4896</v>
       </c>
-      <c r="D108" s="7">
+      <c r="F108" s="7">
         <v>623.99999999999989</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C109" s="7">
+      <c r="C109" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="7">
         <v>500.33724444444448</v>
       </c>
-      <c r="D109" s="7">
+      <c r="F109" s="7">
         <v>322.39999999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C110" s="7">
+      <c r="C110" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E110" s="7">
         <v>282.89706666666666</v>
       </c>
-      <c r="D110" s="7">
+      <c r="F110" s="7">
         <v>136.5</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C111" s="7">
+      <c r="C111" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E111" s="7">
         <v>44.444444444444443</v>
       </c>
-      <c r="D111" s="7">
+      <c r="F111" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C112" s="7">
+      <c r="C112" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="7">
         <v>403.78794666666664</v>
       </c>
-      <c r="D112" s="7">
+      <c r="F112" s="7">
         <v>211.89999999999998</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C113" s="7">
+      <c r="C113" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="7">
         <v>407.74622444444447</v>
       </c>
-      <c r="D113" s="7">
+      <c r="F113" s="7">
         <v>267.14999999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C114" s="7">
+      <c r="C114" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="7">
         <v>305.93713777777776</v>
       </c>
-      <c r="D114" s="7">
+      <c r="F114" s="7">
         <v>187.2</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C115" s="7">
+      <c r="C115" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" s="7">
         <v>440.03371555555555</v>
       </c>
-      <c r="D115" s="7">
+      <c r="F115" s="7">
         <v>200.2</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C116" s="7">
+      <c r="C116" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E116" s="7">
         <v>346.74686666666662</v>
       </c>
-      <c r="D116" s="7">
+      <c r="F116" s="7">
         <v>120.24999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C117" s="7">
+      <c r="C117" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E117" s="7">
         <v>46.222222222222221</v>
       </c>
-      <c r="D117" s="7">
+      <c r="F117" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C118" s="7">
+      <c r="C118" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E118" s="7">
         <v>44.444444444444443</v>
       </c>
-      <c r="D118" s="7">
+      <c r="F118" s="7">
         <v>16.25</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C119" s="8">
+      <c r="C119" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E119" s="8">
         <v>148.44444444444446</v>
       </c>
-      <c r="D119" s="7">
+      <c r="F119" s="7">
         <v>968.6</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C120" s="8">
+      <c r="C120" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E120" s="8">
         <v>111.11111111111111</v>
       </c>
-      <c r="D120" s="7">
+      <c r="F120" s="7">
         <v>725</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C121" s="8">
+      <c r="C121" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E121" s="8">
         <v>290.66666666666669</v>
       </c>
-      <c r="D121" s="7">
+      <c r="F121" s="7">
         <v>1896.5999999999997</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C122" s="8">
+      <c r="C122" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E122" s="8">
         <v>132.44444444444446</v>
       </c>
-      <c r="D122" s="7">
+      <c r="F122" s="7">
         <v>864.19999999999993</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C123" s="8">
+      <c r="C123" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E123" s="8">
         <v>102.22222222222223</v>
       </c>
-      <c r="D123" s="7">
+      <c r="F123" s="7">
         <v>666.99999999999989</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C124" s="8">
+      <c r="C124" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E124" s="8">
         <v>30.222222222222221</v>
       </c>
-      <c r="D124" s="7">
+      <c r="F124" s="7">
         <v>197.2</v>
       </c>
     </row>

</xml_diff>